<commit_message>
Updated training set - removed unnecessary rows
</commit_message>
<xml_diff>
--- a/TrainingData/MiscFiles/TimeSweep100Bar120C.xlsx
+++ b/TrainingData/MiscFiles/TimeSweep100Bar120C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Himendra\Documents\Code\ConfocalImageAnalysis\CO2MachineLearning\TrainingData\MiscFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9577027-8430-40A8-A630-46A4D4813295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B10C1C1-3B71-4068-AFC1-671DD9A6E56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1CD4BD68-6A18-4F23-BCC7-708FEF507E13}"/>
+    <workbookView xWindow="40320" yWindow="525" windowWidth="29010" windowHeight="15450" xr2:uid="{1CD4BD68-6A18-4F23-BCC7-708FEF507E13}"/>
   </bookViews>
   <sheets>
     <sheet name="80-150" sheetId="1" r:id="rId1"/>
@@ -101,8 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -420,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8461008-E9A8-4CB1-AF0B-6338F0DA6B49}">
   <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="H137" sqref="H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +473,7 @@
         <f>B2/MAX(B:B)</f>
         <v>7.0921985815602835E-3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>3925.5</v>
       </c>
       <c r="E2">
@@ -506,13 +505,13 @@
         <v>600</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C66" si="2">B3/MAX(B:B)</f>
+        <f>B3/MAX(B:B)</f>
         <v>1.4184397163120567E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>3265.4</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
@@ -541,13 +540,13 @@
         <v>900</v>
       </c>
       <c r="C4">
-        <f t="shared" si="2"/>
+        <f>B4/MAX(B:B)</f>
         <v>2.1276595744680851E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>2895</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>100</v>
       </c>
       <c r="F4">
@@ -576,13 +575,13 @@
         <v>1200</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f>B5/MAX(B:B)</f>
         <v>2.8368794326241134E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>2822.1</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>100</v>
       </c>
       <c r="F5">
@@ -611,13 +610,13 @@
         <v>1500</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f>B6/MAX(B:B)</f>
         <v>3.5460992907801421E-2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>2542.4</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>100</v>
       </c>
       <c r="F6">
@@ -646,13 +645,13 @@
         <v>1800</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f>B7/MAX(B:B)</f>
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>2326.9</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>100</v>
       </c>
       <c r="F7">
@@ -681,13 +680,13 @@
         <v>2100</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
+        <f>B8/MAX(B:B)</f>
         <v>4.9645390070921988E-2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>2164.4</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>100</v>
       </c>
       <c r="F8">
@@ -716,13 +715,13 @@
         <v>2400</v>
       </c>
       <c r="C9">
-        <f t="shared" si="2"/>
+        <f>B9/MAX(B:B)</f>
         <v>5.6737588652482268E-2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>2034.9</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
@@ -751,13 +750,13 @@
         <v>2700</v>
       </c>
       <c r="C10">
-        <f t="shared" si="2"/>
+        <f>B10/MAX(B:B)</f>
         <v>6.3829787234042548E-2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>1900.2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>100</v>
       </c>
       <c r="F10">
@@ -786,13 +785,13 @@
         <v>3000</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
+        <f>B11/MAX(B:B)</f>
         <v>7.0921985815602842E-2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>1786.2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>100</v>
       </c>
       <c r="F11">
@@ -821,13 +820,13 @@
         <v>3300</v>
       </c>
       <c r="C12">
-        <f t="shared" si="2"/>
+        <f>B12/MAX(B:B)</f>
         <v>7.8014184397163122E-2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>1666.9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>100</v>
       </c>
       <c r="F12">
@@ -856,13 +855,13 @@
         <v>3600</v>
       </c>
       <c r="C13">
-        <f t="shared" si="2"/>
+        <f>B13/MAX(B:B)</f>
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>1581</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>100</v>
       </c>
       <c r="F13">
@@ -891,13 +890,13 @@
         <v>3900</v>
       </c>
       <c r="C14">
-        <f t="shared" si="2"/>
+        <f>B14/MAX(B:B)</f>
         <v>9.2198581560283682E-2</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>1505.5</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>100</v>
       </c>
       <c r="F14">
@@ -926,13 +925,13 @@
         <v>4200</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f>B15/MAX(B:B)</f>
         <v>9.9290780141843976E-2</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>1433.8</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>100</v>
       </c>
       <c r="F15">
@@ -961,13 +960,13 @@
         <v>4500</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f>B16/MAX(B:B)</f>
         <v>0.10638297872340426</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>1372.5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>100</v>
       </c>
       <c r="F16">
@@ -996,13 +995,13 @@
         <v>4800</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f>B17/MAX(B:B)</f>
         <v>0.11347517730496454</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>1318.5</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>100</v>
       </c>
       <c r="F17">
@@ -1031,13 +1030,13 @@
         <v>5100</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f>B18/MAX(B:B)</f>
         <v>0.12056737588652482</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>1268.3</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>100</v>
       </c>
       <c r="F18">
@@ -1066,13 +1065,13 @@
         <v>5400</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f>B19/MAX(B:B)</f>
         <v>0.1276595744680851</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>1197.2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>100</v>
       </c>
       <c r="F19">
@@ -1101,13 +1100,13 @@
         <v>5700</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f>B20/MAX(B:B)</f>
         <v>0.13475177304964539</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>1157.5</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>100</v>
       </c>
       <c r="F20">
@@ -1136,13 +1135,13 @@
         <v>6000</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f>B21/MAX(B:B)</f>
         <v>0.14184397163120568</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>1112.5999999999999</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <v>100</v>
       </c>
       <c r="F21">
@@ -1171,13 +1170,13 @@
         <v>6300</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f>B22/MAX(B:B)</f>
         <v>0.14893617021276595</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>1063.0999999999999</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
         <v>100</v>
       </c>
       <c r="F22">
@@ -1206,13 +1205,13 @@
         <v>6600</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
+        <f>B23/MAX(B:B)</f>
         <v>0.15602836879432624</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>1024.0999999999999</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23">
         <v>100</v>
       </c>
       <c r="F23">
@@ -1241,13 +1240,13 @@
         <v>6900</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f>B24/MAX(B:B)</f>
         <v>0.16312056737588654</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>979.21</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <v>100</v>
       </c>
       <c r="F24">
@@ -1276,13 +1275,13 @@
         <v>7200</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f>B25/MAX(B:B)</f>
         <v>0.1702127659574468</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>959.45</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
         <v>100</v>
       </c>
       <c r="F25">
@@ -1311,13 +1310,13 @@
         <v>7500</v>
       </c>
       <c r="C26">
-        <f t="shared" si="2"/>
+        <f>B26/MAX(B:B)</f>
         <v>0.1773049645390071</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>907.65</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
         <v>100</v>
       </c>
       <c r="F26">
@@ -1346,13 +1345,13 @@
         <v>7800</v>
       </c>
       <c r="C27">
-        <f t="shared" si="2"/>
+        <f>B27/MAX(B:B)</f>
         <v>0.18439716312056736</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>872.9</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27">
         <v>100</v>
       </c>
       <c r="F27">
@@ -1381,13 +1380,13 @@
         <v>8100</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
+        <f>B28/MAX(B:B)</f>
         <v>0.19148936170212766</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>836.19</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28">
         <v>100</v>
       </c>
       <c r="F28">
@@ -1416,13 +1415,13 @@
         <v>8400</v>
       </c>
       <c r="C29">
-        <f t="shared" si="2"/>
+        <f>B29/MAX(B:B)</f>
         <v>0.19858156028368795</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>802.66</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <v>100</v>
       </c>
       <c r="F29">
@@ -1451,13 +1450,13 @@
         <v>8700</v>
       </c>
       <c r="C30">
-        <f t="shared" si="2"/>
+        <f>B30/MAX(B:B)</f>
         <v>0.20567375886524822</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>773.21</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30">
         <v>100</v>
       </c>
       <c r="F30">
@@ -1486,13 +1485,13 @@
         <v>9000</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
+        <f>B31/MAX(B:B)</f>
         <v>0.21276595744680851</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>746.82</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31">
         <v>100</v>
       </c>
       <c r="F31">
@@ -1521,13 +1520,13 @@
         <v>9300</v>
       </c>
       <c r="C32">
-        <f t="shared" si="2"/>
+        <f>B32/MAX(B:B)</f>
         <v>0.21985815602836881</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>727.79</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32">
         <v>100</v>
       </c>
       <c r="F32">
@@ -1556,13 +1555,13 @@
         <v>9600</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
+        <f>B33/MAX(B:B)</f>
         <v>0.22695035460992907</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>730.58</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33">
         <v>100</v>
       </c>
       <c r="F33">
@@ -1591,13 +1590,13 @@
         <v>9900</v>
       </c>
       <c r="C34">
-        <f t="shared" si="2"/>
+        <f>B34/MAX(B:B)</f>
         <v>0.23404255319148937</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>689.66</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34">
         <v>100</v>
       </c>
       <c r="F34">
@@ -1613,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="J34">
-        <f t="shared" ref="J34:J53" si="3">1*PI()*H34^4*D34/2/G34</f>
+        <f t="shared" ref="J34:J53" si="2">1*PI()*H34^4*D34/2/G34</f>
         <v>1.0833153947373683E-2</v>
       </c>
     </row>
@@ -1626,29 +1625,29 @@
         <v>10200</v>
       </c>
       <c r="C35">
+        <f>B35/MAX(B:B)</f>
+        <v>0.24113475177304963</v>
+      </c>
+      <c r="D35">
+        <v>679.38</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35">
+        <v>120</v>
+      </c>
+      <c r="G35">
+        <v>1E-3</v>
+      </c>
+      <c r="H35">
+        <v>0.01</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
         <f t="shared" si="2"/>
-        <v>0.24113475177304963</v>
-      </c>
-      <c r="D35" s="1">
-        <v>679.38</v>
-      </c>
-      <c r="E35" s="1">
-        <v>100</v>
-      </c>
-      <c r="F35">
-        <v>120</v>
-      </c>
-      <c r="G35">
-        <v>1E-3</v>
-      </c>
-      <c r="H35">
-        <v>0.01</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="3"/>
         <v>1.0671676084979168E-2</v>
       </c>
     </row>
@@ -1661,29 +1660,29 @@
         <v>10500</v>
       </c>
       <c r="C36">
+        <f>B36/MAX(B:B)</f>
+        <v>0.24822695035460993</v>
+      </c>
+      <c r="D36">
+        <v>640.28</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36">
+        <v>120</v>
+      </c>
+      <c r="G36">
+        <v>1E-3</v>
+      </c>
+      <c r="H36">
+        <v>0.01</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
         <f t="shared" si="2"/>
-        <v>0.24822695035460993</v>
-      </c>
-      <c r="D36" s="1">
-        <v>640.28</v>
-      </c>
-      <c r="E36" s="1">
-        <v>100</v>
-      </c>
-      <c r="F36">
-        <v>120</v>
-      </c>
-      <c r="G36">
-        <v>1E-3</v>
-      </c>
-      <c r="H36">
-        <v>0.01</v>
-      </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="3"/>
         <v>1.0057494721202362E-2</v>
       </c>
     </row>
@@ -1696,29 +1695,29 @@
         <v>10800</v>
       </c>
       <c r="C37">
+        <f>B37/MAX(B:B)</f>
+        <v>0.25531914893617019</v>
+      </c>
+      <c r="D37">
+        <v>614.54</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37">
+        <v>120</v>
+      </c>
+      <c r="G37">
+        <v>1E-3</v>
+      </c>
+      <c r="H37">
+        <v>0.01</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
         <f t="shared" si="2"/>
-        <v>0.25531914893617019</v>
-      </c>
-      <c r="D37" s="1">
-        <v>614.54</v>
-      </c>
-      <c r="E37" s="1">
-        <v>100</v>
-      </c>
-      <c r="F37">
-        <v>120</v>
-      </c>
-      <c r="G37">
-        <v>1E-3</v>
-      </c>
-      <c r="H37">
-        <v>0.01</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="3"/>
         <v>9.6531717466853562E-3</v>
       </c>
     </row>
@@ -1731,29 +1730,29 @@
         <v>11100</v>
       </c>
       <c r="C38">
+        <f>B38/MAX(B:B)</f>
+        <v>0.26241134751773049</v>
+      </c>
+      <c r="D38">
+        <v>590.26</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38">
+        <v>120</v>
+      </c>
+      <c r="G38">
+        <v>1E-3</v>
+      </c>
+      <c r="H38">
+        <v>0.01</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
         <f t="shared" si="2"/>
-        <v>0.26241134751773049</v>
-      </c>
-      <c r="D38" s="1">
-        <v>590.26</v>
-      </c>
-      <c r="E38" s="1">
-        <v>100</v>
-      </c>
-      <c r="F38">
-        <v>120</v>
-      </c>
-      <c r="G38">
-        <v>1E-3</v>
-      </c>
-      <c r="H38">
-        <v>0.01</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="3"/>
         <v>9.2717823985395565E-3</v>
       </c>
     </row>
@@ -1766,29 +1765,29 @@
         <v>11400</v>
       </c>
       <c r="C39">
+        <f>B39/MAX(B:B)</f>
+        <v>0.26950354609929078</v>
+      </c>
+      <c r="D39">
+        <v>567.09</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39">
+        <v>120</v>
+      </c>
+      <c r="G39">
+        <v>1E-3</v>
+      </c>
+      <c r="H39">
+        <v>0.01</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
         <f t="shared" si="2"/>
-        <v>0.26950354609929078</v>
-      </c>
-      <c r="D39" s="1">
-        <v>567.09</v>
-      </c>
-      <c r="E39" s="1">
-        <v>100</v>
-      </c>
-      <c r="F39">
-        <v>120</v>
-      </c>
-      <c r="G39">
-        <v>1E-3</v>
-      </c>
-      <c r="H39">
-        <v>0.01</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="3"/>
         <v>8.9078288896211784E-3</v>
       </c>
     </row>
@@ -1801,29 +1800,29 @@
         <v>11700</v>
       </c>
       <c r="C40">
+        <f>B40/MAX(B:B)</f>
+        <v>0.27659574468085107</v>
+      </c>
+      <c r="D40">
+        <v>547.95000000000005</v>
+      </c>
+      <c r="E40">
+        <v>100</v>
+      </c>
+      <c r="F40">
+        <v>120</v>
+      </c>
+      <c r="G40">
+        <v>1E-3</v>
+      </c>
+      <c r="H40">
+        <v>0.01</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
         <f t="shared" si="2"/>
-        <v>0.27659574468085107</v>
-      </c>
-      <c r="D40" s="1">
-        <v>547.95000000000005</v>
-      </c>
-      <c r="E40" s="1">
-        <v>100</v>
-      </c>
-      <c r="F40">
-        <v>120</v>
-      </c>
-      <c r="G40">
-        <v>1E-3</v>
-      </c>
-      <c r="H40">
-        <v>0.01</v>
-      </c>
-      <c r="I40">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="3"/>
         <v>8.6071784726726355E-3</v>
       </c>
     </row>
@@ -1836,29 +1835,29 @@
         <v>12000</v>
       </c>
       <c r="C41">
+        <f>B41/MAX(B:B)</f>
+        <v>0.28368794326241137</v>
+      </c>
+      <c r="D41">
+        <v>534.02</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41">
+        <v>120</v>
+      </c>
+      <c r="G41">
+        <v>1E-3</v>
+      </c>
+      <c r="H41">
+        <v>0.01</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="2"/>
-        <v>0.28368794326241137</v>
-      </c>
-      <c r="D41" s="1">
-        <v>534.02</v>
-      </c>
-      <c r="E41" s="1">
-        <v>100</v>
-      </c>
-      <c r="F41">
-        <v>120</v>
-      </c>
-      <c r="G41">
-        <v>1E-3</v>
-      </c>
-      <c r="H41">
-        <v>0.01</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="3"/>
         <v>8.3883665443501062E-3</v>
       </c>
     </row>
@@ -1871,29 +1870,29 @@
         <v>12300</v>
       </c>
       <c r="C42">
+        <f>B42/MAX(B:B)</f>
+        <v>0.29078014184397161</v>
+      </c>
+      <c r="D42">
+        <v>516.29999999999995</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42">
+        <v>120</v>
+      </c>
+      <c r="G42">
+        <v>1E-3</v>
+      </c>
+      <c r="H42">
+        <v>0.01</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="2"/>
-        <v>0.29078014184397161</v>
-      </c>
-      <c r="D42" s="1">
-        <v>516.29999999999995</v>
-      </c>
-      <c r="E42" s="1">
-        <v>100</v>
-      </c>
-      <c r="F42">
-        <v>120</v>
-      </c>
-      <c r="G42">
-        <v>1E-3</v>
-      </c>
-      <c r="H42">
-        <v>0.01</v>
-      </c>
-      <c r="I42">
-        <v>1</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="3"/>
         <v>8.1100214352420492E-3</v>
       </c>
     </row>
@@ -1906,29 +1905,29 @@
         <v>12600</v>
       </c>
       <c r="C43">
+        <f>B43/MAX(B:B)</f>
+        <v>0.2978723404255319</v>
+      </c>
+      <c r="D43">
+        <v>508.8</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43">
+        <v>120</v>
+      </c>
+      <c r="G43">
+        <v>1E-3</v>
+      </c>
+      <c r="H43">
+        <v>0.01</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
         <f t="shared" si="2"/>
-        <v>0.2978723404255319</v>
-      </c>
-      <c r="D43" s="1">
-        <v>508.8</v>
-      </c>
-      <c r="E43" s="1">
-        <v>100</v>
-      </c>
-      <c r="F43">
-        <v>120</v>
-      </c>
-      <c r="G43">
-        <v>1E-3</v>
-      </c>
-      <c r="H43">
-        <v>0.01</v>
-      </c>
-      <c r="I43">
-        <v>1</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="3"/>
         <v>7.9922117107324338E-3</v>
       </c>
     </row>
@@ -1941,29 +1940,29 @@
         <v>12900</v>
       </c>
       <c r="C44">
+        <f>B44/MAX(B:B)</f>
+        <v>0.30496453900709219</v>
+      </c>
+      <c r="D44">
+        <v>494.45</v>
+      </c>
+      <c r="E44">
+        <v>100</v>
+      </c>
+      <c r="F44">
+        <v>120</v>
+      </c>
+      <c r="G44">
+        <v>1E-3</v>
+      </c>
+      <c r="H44">
+        <v>0.01</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
         <f t="shared" si="2"/>
-        <v>0.30496453900709219</v>
-      </c>
-      <c r="D44" s="1">
-        <v>494.45</v>
-      </c>
-      <c r="E44" s="1">
-        <v>100</v>
-      </c>
-      <c r="F44">
-        <v>120</v>
-      </c>
-      <c r="G44">
-        <v>1E-3</v>
-      </c>
-      <c r="H44">
-        <v>0.01</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="3"/>
         <v>7.7668024378373651E-3</v>
       </c>
     </row>
@@ -1976,29 +1975,29 @@
         <v>13200</v>
       </c>
       <c r="C45">
+        <f>B45/MAX(B:B)</f>
+        <v>0.31205673758865249</v>
+      </c>
+      <c r="D45">
+        <v>472.79</v>
+      </c>
+      <c r="E45">
+        <v>100</v>
+      </c>
+      <c r="F45">
+        <v>120</v>
+      </c>
+      <c r="G45">
+        <v>1E-3</v>
+      </c>
+      <c r="H45">
+        <v>0.01</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
         <f t="shared" si="2"/>
-        <v>0.31205673758865249</v>
-      </c>
-      <c r="D45" s="1">
-        <v>472.79</v>
-      </c>
-      <c r="E45" s="1">
-        <v>100</v>
-      </c>
-      <c r="F45">
-        <v>120</v>
-      </c>
-      <c r="G45">
-        <v>1E-3</v>
-      </c>
-      <c r="H45">
-        <v>0.01</v>
-      </c>
-      <c r="I45">
-        <v>1</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="3"/>
         <v>7.4265679534535915E-3</v>
       </c>
     </row>
@@ -2011,29 +2010,29 @@
         <v>13500</v>
       </c>
       <c r="C46">
+        <f>B46/MAX(B:B)</f>
+        <v>0.31914893617021278</v>
+      </c>
+      <c r="D46">
+        <v>470.53</v>
+      </c>
+      <c r="E46">
+        <v>100</v>
+      </c>
+      <c r="F46">
+        <v>120</v>
+      </c>
+      <c r="G46">
+        <v>1E-3</v>
+      </c>
+      <c r="H46">
+        <v>0.01</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
         <f t="shared" si="2"/>
-        <v>0.31914893617021278</v>
-      </c>
-      <c r="D46" s="1">
-        <v>470.53</v>
-      </c>
-      <c r="E46" s="1">
-        <v>100</v>
-      </c>
-      <c r="F46">
-        <v>120</v>
-      </c>
-      <c r="G46">
-        <v>1E-3</v>
-      </c>
-      <c r="H46">
-        <v>0.01</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="3"/>
         <v>7.3910679564680257E-3</v>
       </c>
     </row>
@@ -2046,29 +2045,29 @@
         <v>13800</v>
       </c>
       <c r="C47">
+        <f>B47/MAX(B:B)</f>
+        <v>0.32624113475177308</v>
+      </c>
+      <c r="D47">
+        <v>460.69</v>
+      </c>
+      <c r="E47">
+        <v>100</v>
+      </c>
+      <c r="F47">
+        <v>120</v>
+      </c>
+      <c r="G47">
+        <v>1E-3</v>
+      </c>
+      <c r="H47">
+        <v>0.01</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
         <f t="shared" si="2"/>
-        <v>0.32624113475177308</v>
-      </c>
-      <c r="D47" s="1">
-        <v>460.69</v>
-      </c>
-      <c r="E47" s="1">
-        <v>100</v>
-      </c>
-      <c r="F47">
-        <v>120</v>
-      </c>
-      <c r="G47">
-        <v>1E-3</v>
-      </c>
-      <c r="H47">
-        <v>0.01</v>
-      </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="3"/>
         <v>7.236501597911409E-3</v>
       </c>
     </row>
@@ -2081,29 +2080,29 @@
         <v>14100</v>
       </c>
       <c r="C48">
+        <f>B48/MAX(B:B)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D48">
+        <v>449.75</v>
+      </c>
+      <c r="E48">
+        <v>100</v>
+      </c>
+      <c r="F48">
+        <v>120</v>
+      </c>
+      <c r="G48">
+        <v>1E-3</v>
+      </c>
+      <c r="H48">
+        <v>0.01</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D48" s="1">
-        <v>449.75</v>
-      </c>
-      <c r="E48" s="1">
-        <v>100</v>
-      </c>
-      <c r="F48">
-        <v>120</v>
-      </c>
-      <c r="G48">
-        <v>1E-3</v>
-      </c>
-      <c r="H48">
-        <v>0.01</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="3"/>
         <v>7.0646564797600475E-3</v>
       </c>
     </row>
@@ -2116,29 +2115,29 @@
         <v>14400</v>
       </c>
       <c r="C49">
+        <f>B49/MAX(B:B)</f>
+        <v>0.34042553191489361</v>
+      </c>
+      <c r="D49">
+        <v>448.54</v>
+      </c>
+      <c r="E49">
+        <v>100</v>
+      </c>
+      <c r="F49">
+        <v>120</v>
+      </c>
+      <c r="G49">
+        <v>1E-3</v>
+      </c>
+      <c r="H49">
+        <v>0.01</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
         <f t="shared" si="2"/>
-        <v>0.34042553191489361</v>
-      </c>
-      <c r="D49" s="1">
-        <v>448.54</v>
-      </c>
-      <c r="E49" s="1">
-        <v>100</v>
-      </c>
-      <c r="F49">
-        <v>120</v>
-      </c>
-      <c r="G49">
-        <v>1E-3</v>
-      </c>
-      <c r="H49">
-        <v>0.01</v>
-      </c>
-      <c r="I49">
-        <v>1</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="3"/>
         <v>7.0456498442058287E-3</v>
       </c>
     </row>
@@ -2151,29 +2150,29 @@
         <v>14700</v>
       </c>
       <c r="C50">
+        <f>B50/MAX(B:B)</f>
+        <v>0.3475177304964539</v>
+      </c>
+      <c r="D50">
+        <v>433.41</v>
+      </c>
+      <c r="E50">
+        <v>100</v>
+      </c>
+      <c r="F50">
+        <v>120</v>
+      </c>
+      <c r="G50">
+        <v>1E-3</v>
+      </c>
+      <c r="H50">
+        <v>0.01</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
         <f t="shared" si="2"/>
-        <v>0.3475177304964539</v>
-      </c>
-      <c r="D50" s="1">
-        <v>433.41</v>
-      </c>
-      <c r="E50" s="1">
-        <v>100</v>
-      </c>
-      <c r="F50">
-        <v>120</v>
-      </c>
-      <c r="G50">
-        <v>1E-3</v>
-      </c>
-      <c r="H50">
-        <v>0.01</v>
-      </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="3"/>
         <v>6.807988359961761E-3</v>
       </c>
     </row>
@@ -2186,29 +2185,29 @@
         <v>15000</v>
       </c>
       <c r="C51">
+        <f>B51/MAX(B:B)</f>
+        <v>0.3546099290780142</v>
+      </c>
+      <c r="D51">
+        <v>425.84</v>
+      </c>
+      <c r="E51">
+        <v>100</v>
+      </c>
+      <c r="F51">
+        <v>120</v>
+      </c>
+      <c r="G51">
+        <v>1E-3</v>
+      </c>
+      <c r="H51">
+        <v>0.01</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
         <f t="shared" si="2"/>
-        <v>0.3546099290780142</v>
-      </c>
-      <c r="D51" s="1">
-        <v>425.84</v>
-      </c>
-      <c r="E51" s="1">
-        <v>100</v>
-      </c>
-      <c r="F51">
-        <v>120</v>
-      </c>
-      <c r="G51">
-        <v>1E-3</v>
-      </c>
-      <c r="H51">
-        <v>0.01</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="3"/>
         <v>6.6890790780233869E-3</v>
       </c>
     </row>
@@ -2221,29 +2220,29 @@
         <v>15300</v>
       </c>
       <c r="C52">
+        <f>B52/MAX(B:B)</f>
+        <v>0.36170212765957449</v>
+      </c>
+      <c r="D52">
+        <v>420.79</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="F52">
+        <v>120</v>
+      </c>
+      <c r="G52">
+        <v>1E-3</v>
+      </c>
+      <c r="H52">
+        <v>0.01</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
         <f t="shared" si="2"/>
-        <v>0.36170212765957449</v>
-      </c>
-      <c r="D52" s="1">
-        <v>420.79</v>
-      </c>
-      <c r="E52" s="1">
-        <v>100</v>
-      </c>
-      <c r="F52">
-        <v>120</v>
-      </c>
-      <c r="G52">
-        <v>1E-3</v>
-      </c>
-      <c r="H52">
-        <v>0.01</v>
-      </c>
-      <c r="I52">
-        <v>1</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="3"/>
         <v>6.6097538635202452E-3</v>
       </c>
     </row>
@@ -2256,29 +2255,29 @@
         <v>15600</v>
       </c>
       <c r="C53">
+        <f>B53/MAX(B:B)</f>
+        <v>0.36879432624113473</v>
+      </c>
+      <c r="D53">
+        <v>416.65</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53">
+        <v>120</v>
+      </c>
+      <c r="G53">
+        <v>1E-3</v>
+      </c>
+      <c r="H53">
+        <v>0.01</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
         <f t="shared" si="2"/>
-        <v>0.36879432624113473</v>
-      </c>
-      <c r="D53" s="1">
-        <v>416.65</v>
-      </c>
-      <c r="E53" s="1">
-        <v>100</v>
-      </c>
-      <c r="F53">
-        <v>120</v>
-      </c>
-      <c r="G53">
-        <v>1E-3</v>
-      </c>
-      <c r="H53">
-        <v>0.01</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="3"/>
         <v>6.5447228955909358E-3</v>
       </c>
     </row>
@@ -2287,17 +2286,17 @@
         <v>265</v>
       </c>
       <c r="B54">
-        <f t="shared" ref="B54:B117" si="4">A54*60</f>
+        <f t="shared" ref="B54:B117" si="3">A54*60</f>
         <v>15900</v>
       </c>
       <c r="C54">
-        <f t="shared" si="2"/>
+        <f>B54/MAX(B:B)</f>
         <v>0.37588652482269502</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54">
         <v>407.8</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54">
         <v>100</v>
       </c>
       <c r="F54">
@@ -2313,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="J54">
-        <f t="shared" ref="J54:J117" si="5">1*PI()*H54^4*D54/2/G54</f>
+        <f t="shared" ref="J54:J117" si="4">1*PI()*H54^4*D54/2/G54</f>
         <v>6.4057074206695886E-3</v>
       </c>
     </row>
@@ -2322,17 +2321,17 @@
         <v>270</v>
       </c>
       <c r="B55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16200</v>
       </c>
       <c r="C55">
-        <f t="shared" si="2"/>
+        <f>B55/MAX(B:B)</f>
         <v>0.38297872340425532</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55">
         <v>400.67</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55">
         <v>100</v>
       </c>
       <c r="F55">
@@ -2348,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="J55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.2937096425691123E-3</v>
       </c>
     </row>
@@ -2357,17 +2356,17 @@
         <v>275</v>
       </c>
       <c r="B56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16500</v>
       </c>
       <c r="C56">
-        <f t="shared" si="2"/>
+        <f>B56/MAX(B:B)</f>
         <v>0.39007092198581561</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56">
         <v>402.85</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56">
         <v>100</v>
       </c>
       <c r="F56">
@@ -2383,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="J56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.3279530024932416E-3</v>
       </c>
     </row>
@@ -2392,17 +2391,17 @@
         <v>280</v>
       </c>
       <c r="B57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16800</v>
       </c>
       <c r="C57">
-        <f t="shared" si="2"/>
+        <f>B57/MAX(B:B)</f>
         <v>0.3971631205673759</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57">
         <v>382.26</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57">
         <v>100</v>
       </c>
       <c r="F57">
@@ -2418,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="J57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.0045260388061714E-3</v>
       </c>
     </row>
@@ -2427,17 +2426,17 @@
         <v>285</v>
       </c>
       <c r="B58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17100</v>
       </c>
       <c r="C58">
-        <f t="shared" si="2"/>
+        <f>B58/MAX(B:B)</f>
         <v>0.40425531914893614</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58">
         <v>373.58</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58">
         <v>100</v>
       </c>
       <c r="F58">
@@ -2453,7 +2452,7 @@
         <v>1</v>
       </c>
       <c r="J58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.868180917640374E-3</v>
       </c>
     </row>
@@ -2462,17 +2461,17 @@
         <v>290</v>
       </c>
       <c r="B59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17400</v>
       </c>
       <c r="C59">
-        <f t="shared" si="2"/>
+        <f>B59/MAX(B:B)</f>
         <v>0.41134751773049644</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59">
         <v>367.66</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59">
         <v>100</v>
       </c>
       <c r="F59">
@@ -2488,7 +2487,7 @@
         <v>1</v>
       </c>
       <c r="J59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.7751897750941174E-3</v>
       </c>
     </row>
@@ -2497,17 +2496,17 @@
         <v>295</v>
       </c>
       <c r="B60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17700</v>
       </c>
       <c r="C60">
-        <f t="shared" si="2"/>
+        <f>B60/MAX(B:B)</f>
         <v>0.41843971631205673</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60">
         <v>376.64</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60">
         <v>100</v>
       </c>
       <c r="F60">
@@ -2523,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="J60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.9162472852402979E-3</v>
       </c>
     </row>
@@ -2532,17 +2531,17 @@
         <v>300</v>
       </c>
       <c r="B61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18000</v>
       </c>
       <c r="C61">
-        <f t="shared" si="2"/>
+        <f>B61/MAX(B:B)</f>
         <v>0.42553191489361702</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61">
         <v>365.43</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61">
         <v>100</v>
       </c>
       <c r="F61">
@@ -2558,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="J61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.7401610170065903E-3</v>
       </c>
     </row>
@@ -2567,17 +2566,17 @@
         <v>305</v>
       </c>
       <c r="B62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18300</v>
       </c>
       <c r="C62">
-        <f t="shared" si="2"/>
+        <f>B62/MAX(B:B)</f>
         <v>0.43262411347517732</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62">
         <v>355.18</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62">
         <v>100</v>
       </c>
       <c r="F62">
@@ -2593,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="J62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.5791543935101136E-3</v>
       </c>
     </row>
@@ -2602,17 +2601,17 @@
         <v>310</v>
       </c>
       <c r="B63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18600</v>
       </c>
       <c r="C63">
-        <f t="shared" si="2"/>
+        <f>B63/MAX(B:B)</f>
         <v>0.43971631205673761</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63">
         <v>332.46</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63">
         <v>100</v>
       </c>
       <c r="F63">
@@ -2628,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="J63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.2222694680623127E-3</v>
       </c>
     </row>
@@ -2637,17 +2636,17 @@
         <v>315</v>
       </c>
       <c r="B64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18900</v>
       </c>
       <c r="C64">
-        <f t="shared" si="2"/>
+        <f>B64/MAX(B:B)</f>
         <v>0.44680851063829785</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64">
         <v>330.23</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64">
         <v>100</v>
       </c>
       <c r="F64">
@@ -2663,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="J64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.1872407099747865E-3</v>
       </c>
     </row>
@@ -2672,17 +2671,17 @@
         <v>320</v>
       </c>
       <c r="B65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19200</v>
       </c>
       <c r="C65">
-        <f t="shared" si="2"/>
+        <f>B65/MAX(B:B)</f>
         <v>0.45390070921985815</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65">
         <v>329.81</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65">
         <v>100</v>
       </c>
       <c r="F65">
@@ -2698,7 +2697,7 @@
         <v>1</v>
       </c>
       <c r="J65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.1806433654022479E-3</v>
       </c>
     </row>
@@ -2707,17 +2706,17 @@
         <v>325</v>
       </c>
       <c r="B66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19500</v>
       </c>
       <c r="C66">
-        <f t="shared" si="2"/>
+        <f>B66/MAX(B:B)</f>
         <v>0.46099290780141844</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66">
         <v>318.20999999999998</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66">
         <v>100</v>
       </c>
       <c r="F66">
@@ -2733,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="J66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.9984309914940404E-3</v>
       </c>
     </row>
@@ -2742,17 +2741,17 @@
         <v>330</v>
       </c>
       <c r="B67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19800</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" si="6">B67/MAX(B:B)</f>
+        <f>B67/MAX(B:B)</f>
         <v>0.46808510638297873</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67">
         <v>312.97000000000003</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67">
         <v>100</v>
       </c>
       <c r="F67">
@@ -2768,7 +2767,7 @@
         <v>1</v>
       </c>
       <c r="J67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.9161212639699881E-3</v>
       </c>
     </row>
@@ -2777,17 +2776,17 @@
         <v>335</v>
       </c>
       <c r="B68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20100</v>
       </c>
       <c r="C68">
-        <f t="shared" si="6"/>
+        <f>B68/MAX(B:B)</f>
         <v>0.47517730496453903</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68">
         <v>308.95999999999998</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68">
         <v>100</v>
       </c>
       <c r="F68">
@@ -2803,7 +2802,7 @@
         <v>1</v>
       </c>
       <c r="J68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.853132331265512E-3</v>
       </c>
     </row>
@@ -2812,17 +2811,17 @@
         <v>340</v>
       </c>
       <c r="B69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20400</v>
       </c>
       <c r="C69">
-        <f t="shared" si="6"/>
+        <f>B69/MAX(B:B)</f>
         <v>0.48226950354609927</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69">
         <v>303.56</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69">
         <v>100</v>
       </c>
       <c r="F69">
@@ -2838,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="J69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.7683093296185877E-3</v>
       </c>
     </row>
@@ -2847,17 +2846,17 @@
         <v>345</v>
       </c>
       <c r="B70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20700</v>
       </c>
       <c r="C70">
-        <f t="shared" si="6"/>
+        <f>B70/MAX(B:B)</f>
         <v>0.48936170212765956</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70">
         <v>301.57</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70">
         <v>100</v>
       </c>
       <c r="F70">
@@ -2873,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="J70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.7370504827153699E-3</v>
       </c>
     </row>
@@ -2882,17 +2881,17 @@
         <v>350</v>
       </c>
       <c r="B71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21000</v>
       </c>
       <c r="C71">
-        <f t="shared" si="6"/>
+        <f>B71/MAX(B:B)</f>
         <v>0.49645390070921985</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71">
         <v>297.72000000000003</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71">
         <v>100</v>
       </c>
       <c r="F71">
@@ -2908,7 +2907,7 @@
         <v>1</v>
       </c>
       <c r="J71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.6765748241337666E-3</v>
       </c>
     </row>
@@ -2917,17 +2916,17 @@
         <v>355</v>
       </c>
       <c r="B72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21300</v>
       </c>
       <c r="C72">
-        <f t="shared" si="6"/>
+        <f>B72/MAX(B:B)</f>
         <v>0.50354609929078009</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72">
         <v>294.18</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72">
         <v>100</v>
       </c>
       <c r="F72">
@@ -2943,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="J72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.6209686341652269E-3</v>
       </c>
     </row>
@@ -2952,17 +2951,17 @@
         <v>360</v>
       </c>
       <c r="B73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21600</v>
       </c>
       <c r="C73">
-        <f t="shared" si="6"/>
+        <f>B73/MAX(B:B)</f>
         <v>0.51063829787234039</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73">
         <v>290.86</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73">
         <v>100</v>
       </c>
       <c r="F73">
@@ -2978,7 +2977,7 @@
         <v>1</v>
       </c>
       <c r="J73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.5688181961156364E-3</v>
       </c>
     </row>
@@ -2987,17 +2986,17 @@
         <v>365</v>
       </c>
       <c r="B74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21900</v>
       </c>
       <c r="C74">
-        <f t="shared" si="6"/>
+        <f>B74/MAX(B:B)</f>
         <v>0.51773049645390068</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74">
         <v>287.54000000000002</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74">
         <v>100</v>
       </c>
       <c r="F74">
@@ -3013,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="J74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.516667758066046E-3</v>
       </c>
     </row>
@@ -3022,17 +3021,17 @@
         <v>370</v>
       </c>
       <c r="B75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22200</v>
       </c>
       <c r="C75">
-        <f t="shared" si="6"/>
+        <f>B75/MAX(B:B)</f>
         <v>0.52482269503546097</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75">
         <v>283.98</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75">
         <v>100</v>
       </c>
       <c r="F75">
@@ -3048,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="J75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.4607474088321471E-3</v>
       </c>
     </row>
@@ -3057,17 +3056,17 @@
         <v>375</v>
       </c>
       <c r="B76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22500</v>
       </c>
       <c r="C76">
-        <f t="shared" si="6"/>
+        <f>B76/MAX(B:B)</f>
         <v>0.53191489361702127</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76">
         <v>280.61</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76">
         <v>100</v>
       </c>
       <c r="F76">
@@ -3083,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="J76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.4078115726191597E-3</v>
       </c>
     </row>
@@ -3092,17 +3091,17 @@
         <v>380</v>
       </c>
       <c r="B77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22800</v>
       </c>
       <c r="C77">
-        <f t="shared" si="6"/>
+        <f>B77/MAX(B:B)</f>
         <v>0.53900709219858156</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77">
         <v>277.16000000000003</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77">
         <v>100</v>
       </c>
       <c r="F77">
@@ -3118,7 +3117,7 @@
         <v>1</v>
       </c>
       <c r="J77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.353619099344736E-3</v>
       </c>
     </row>
@@ -3127,17 +3126,17 @@
         <v>385</v>
       </c>
       <c r="B78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23100</v>
       </c>
       <c r="C78">
-        <f t="shared" si="6"/>
+        <f>B78/MAX(B:B)</f>
         <v>0.54609929078014185</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78">
         <v>274.56</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78">
         <v>100</v>
       </c>
       <c r="F78">
@@ -3153,7 +3152,7 @@
         <v>1</v>
       </c>
       <c r="J78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.3127783948480681E-3</v>
       </c>
     </row>
@@ -3162,17 +3161,17 @@
         <v>390</v>
       </c>
       <c r="B79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23400</v>
       </c>
       <c r="C79">
-        <f t="shared" si="6"/>
+        <f>B79/MAX(B:B)</f>
         <v>0.55319148936170215</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79">
         <v>270.70999999999998</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79">
         <v>100</v>
       </c>
       <c r="F79">
@@ -3188,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="J79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.2523027362664639E-3</v>
       </c>
     </row>
@@ -3197,17 +3196,17 @@
         <v>395</v>
       </c>
       <c r="B80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23700</v>
       </c>
       <c r="C80">
-        <f t="shared" si="6"/>
+        <f>B80/MAX(B:B)</f>
         <v>0.56028368794326244</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80">
         <v>268.45</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80">
         <v>100</v>
       </c>
       <c r="F80">
@@ -3223,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="J80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.2168027392808999E-3</v>
       </c>
     </row>
@@ -3232,17 +3231,17 @@
         <v>400</v>
       </c>
       <c r="B81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24000</v>
       </c>
       <c r="C81">
-        <f t="shared" si="6"/>
+        <f>B81/MAX(B:B)</f>
         <v>0.56737588652482274</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81">
         <v>265.48</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81">
         <v>100</v>
       </c>
       <c r="F81">
@@ -3258,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="J81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.1701500883750912E-3</v>
       </c>
     </row>
@@ -3267,17 +3266,17 @@
         <v>405</v>
       </c>
       <c r="B82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24300</v>
       </c>
       <c r="C82">
-        <f t="shared" si="6"/>
+        <f>B82/MAX(B:B)</f>
         <v>0.57446808510638303</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82">
         <v>261.37</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82">
         <v>100</v>
       </c>
       <c r="F82">
@@ -3293,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="J82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.1055903593438213E-3</v>
       </c>
     </row>
@@ -3302,17 +3301,17 @@
         <v>410</v>
       </c>
       <c r="B83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24600</v>
       </c>
       <c r="C83">
-        <f t="shared" si="6"/>
+        <f>B83/MAX(B:B)</f>
         <v>0.58156028368794321</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83">
         <v>258.94</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83">
         <v>100</v>
       </c>
       <c r="F83">
@@ -3328,7 +3327,7 @@
         <v>1</v>
       </c>
       <c r="J83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.0674200086027049E-3</v>
       </c>
     </row>
@@ -3337,17 +3336,17 @@
         <v>415</v>
       </c>
       <c r="B84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24900</v>
       </c>
       <c r="C84">
-        <f t="shared" si="6"/>
+        <f>B84/MAX(B:B)</f>
         <v>0.58865248226950351</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84">
         <v>256.61</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84">
         <v>100</v>
       </c>
       <c r="F84">
@@ -3363,7 +3362,7 @@
         <v>1</v>
       </c>
       <c r="J84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.030820454188384E-3</v>
       </c>
     </row>
@@ -3372,17 +3371,17 @@
         <v>420</v>
       </c>
       <c r="B85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25200</v>
       </c>
       <c r="C85">
-        <f t="shared" si="6"/>
+        <f>B85/MAX(B:B)</f>
         <v>0.5957446808510638</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85">
         <v>253.46</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85">
         <v>100</v>
       </c>
       <c r="F85">
@@ -3398,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="J85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.9813403698943442E-3</v>
       </c>
     </row>
@@ -3407,17 +3406,17 @@
         <v>425</v>
       </c>
       <c r="B86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25500</v>
       </c>
       <c r="C86">
-        <f t="shared" si="6"/>
+        <f>B86/MAX(B:B)</f>
         <v>0.6028368794326241</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86">
         <v>250.72</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86">
         <v>100</v>
       </c>
       <c r="F86">
@@ -3433,7 +3432,7 @@
         <v>1</v>
       </c>
       <c r="J86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.9383005505401643E-3</v>
       </c>
     </row>
@@ -3442,17 +3441,17 @@
         <v>430</v>
       </c>
       <c r="B87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25800</v>
       </c>
       <c r="C87">
-        <f t="shared" si="6"/>
+        <f>B87/MAX(B:B)</f>
         <v>0.60992907801418439</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87">
         <v>247.19</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87">
         <v>100</v>
       </c>
       <c r="F87">
@@ -3468,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="J87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.882851440204305E-3</v>
       </c>
     </row>
@@ -3477,17 +3476,17 @@
         <v>435</v>
       </c>
       <c r="B88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26100</v>
       </c>
       <c r="C88">
-        <f t="shared" si="6"/>
+        <f>B88/MAX(B:B)</f>
         <v>0.61702127659574468</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88">
         <v>245.36</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E88">
         <v>100</v>
       </c>
       <c r="F88">
@@ -3503,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="J88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.8541058674239578E-3</v>
       </c>
     </row>
@@ -3512,17 +3511,17 @@
         <v>440</v>
       </c>
       <c r="B89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26400</v>
       </c>
       <c r="C89">
-        <f t="shared" si="6"/>
+        <f>B89/MAX(B:B)</f>
         <v>0.62411347517730498</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89">
         <v>244.36</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E89">
         <v>100</v>
       </c>
       <c r="F89">
@@ -3538,7 +3537,7 @@
         <v>1</v>
       </c>
       <c r="J89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.8383979041560095E-3</v>
       </c>
     </row>
@@ -3547,17 +3546,17 @@
         <v>445</v>
       </c>
       <c r="B90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26700</v>
       </c>
       <c r="C90">
-        <f t="shared" si="6"/>
+        <f>B90/MAX(B:B)</f>
         <v>0.63120567375886527</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90">
         <v>242.71</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E90">
         <v>100</v>
       </c>
       <c r="F90">
@@ -3573,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="J90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.8124797647638934E-3</v>
       </c>
     </row>
@@ -3582,17 +3581,17 @@
         <v>450</v>
       </c>
       <c r="B91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27000</v>
       </c>
       <c r="C91">
-        <f t="shared" si="6"/>
+        <f>B91/MAX(B:B)</f>
         <v>0.63829787234042556</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91">
         <v>236.73</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E91">
         <v>100</v>
       </c>
       <c r="F91">
@@ -3608,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="J91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.7185461444215581E-3</v>
       </c>
     </row>
@@ -3617,17 +3616,17 @@
         <v>455</v>
       </c>
       <c r="B92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27300</v>
       </c>
       <c r="C92">
-        <f t="shared" si="6"/>
+        <f>B92/MAX(B:B)</f>
         <v>0.64539007092198586</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92">
         <v>233.95</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E92">
         <v>100</v>
       </c>
       <c r="F92">
@@ -3643,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="J92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.6748780065366604E-3</v>
       </c>
     </row>
@@ -3652,17 +3651,17 @@
         <v>460</v>
       </c>
       <c r="B93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27600</v>
       </c>
       <c r="C93">
-        <f t="shared" si="6"/>
+        <f>B93/MAX(B:B)</f>
         <v>0.65248226950354615</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93">
         <v>230.56</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E93">
         <v>100</v>
       </c>
       <c r="F93">
@@ -3678,7 +3677,7 @@
         <v>1</v>
       </c>
       <c r="J93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.6216280110583131E-3</v>
       </c>
     </row>
@@ -3687,17 +3686,17 @@
         <v>465</v>
       </c>
       <c r="B94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27900</v>
       </c>
       <c r="C94">
-        <f t="shared" si="6"/>
+        <f>B94/MAX(B:B)</f>
         <v>0.65957446808510634</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94">
         <v>227.91</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E94">
         <v>100</v>
       </c>
       <c r="F94">
@@ -3713,7 +3712,7 @@
         <v>1</v>
       </c>
       <c r="J94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.5800019083982487E-3</v>
       </c>
     </row>
@@ -3722,17 +3721,17 @@
         <v>470</v>
       </c>
       <c r="B95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28200</v>
       </c>
       <c r="C95">
-        <f t="shared" si="6"/>
+        <f>B95/MAX(B:B)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95">
         <v>225.56</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E95">
         <v>100</v>
       </c>
       <c r="F95">
@@ -3748,7 +3747,7 @@
         <v>1</v>
       </c>
       <c r="J95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.5430881947185688E-3</v>
       </c>
     </row>
@@ -3757,17 +3756,17 @@
         <v>475</v>
       </c>
       <c r="B96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28500</v>
       </c>
       <c r="C96">
-        <f t="shared" si="6"/>
+        <f>B96/MAX(B:B)</f>
         <v>0.67375886524822692</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96">
         <v>221.45</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96">
         <v>100</v>
       </c>
       <c r="F96">
@@ -3783,7 +3782,7 @@
         <v>1</v>
       </c>
       <c r="J96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.478528465687298E-3</v>
       </c>
     </row>
@@ -3792,17 +3791,17 @@
         <v>480</v>
       </c>
       <c r="B97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28800</v>
       </c>
       <c r="C97">
-        <f t="shared" si="6"/>
+        <f>B97/MAX(B:B)</f>
         <v>0.68085106382978722</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97">
         <v>217.93</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E97">
         <v>100</v>
       </c>
       <c r="F97">
@@ -3818,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="J97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.4232364349841178E-3</v>
       </c>
     </row>
@@ -3827,17 +3826,17 @@
         <v>485</v>
       </c>
       <c r="B98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>29100</v>
       </c>
       <c r="C98">
-        <f t="shared" si="6"/>
+        <f>B98/MAX(B:B)</f>
         <v>0.68794326241134751</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98">
         <v>215.87</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E98">
         <v>100</v>
       </c>
       <c r="F98">
@@ -3853,7 +3852,7 @@
         <v>1</v>
       </c>
       <c r="J98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.3908780306521431E-3</v>
       </c>
     </row>
@@ -3862,17 +3861,17 @@
         <v>490</v>
       </c>
       <c r="B99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>29400</v>
       </c>
       <c r="C99">
-        <f t="shared" si="6"/>
+        <f>B99/MAX(B:B)</f>
         <v>0.69503546099290781</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99">
         <v>214.56</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E99">
         <v>100</v>
       </c>
       <c r="F99">
@@ -3888,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="J99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.37030059877113E-3</v>
       </c>
     </row>
@@ -3897,17 +3896,17 @@
         <v>495</v>
       </c>
       <c r="B100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>29700</v>
       </c>
       <c r="C100">
-        <f t="shared" si="6"/>
+        <f>B100/MAX(B:B)</f>
         <v>0.7021276595744681</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100">
         <v>212.76</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E100">
         <v>100</v>
       </c>
       <c r="F100">
@@ -3923,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="J100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.3420262648888215E-3</v>
       </c>
     </row>
@@ -3932,17 +3931,17 @@
         <v>500</v>
       </c>
       <c r="B101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30000</v>
       </c>
       <c r="C101">
-        <f t="shared" si="6"/>
+        <f>B101/MAX(B:B)</f>
         <v>0.70921985815602839</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101">
         <v>210.65</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101">
         <v>100</v>
       </c>
       <c r="F101">
@@ -3958,7 +3957,7 @@
         <v>1</v>
       </c>
       <c r="J101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.3088824623934495E-3</v>
       </c>
     </row>
@@ -3967,17 +3966,17 @@
         <v>505</v>
       </c>
       <c r="B102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30300</v>
       </c>
       <c r="C102">
-        <f t="shared" si="6"/>
+        <f>B102/MAX(B:B)</f>
         <v>0.71631205673758869</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102">
         <v>208.64</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102">
         <v>100</v>
       </c>
       <c r="F102">
@@ -3993,7 +3992,7 @@
         <v>1</v>
       </c>
       <c r="J102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2773094562248721E-3</v>
       </c>
     </row>
@@ -4002,17 +4001,17 @@
         <v>510</v>
       </c>
       <c r="B103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30600</v>
       </c>
       <c r="C103">
-        <f t="shared" si="6"/>
+        <f>B103/MAX(B:B)</f>
         <v>0.72340425531914898</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103">
         <v>206.98</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E103">
         <v>100</v>
       </c>
       <c r="F103">
@@ -4028,7 +4027,7 @@
         <v>1</v>
       </c>
       <c r="J103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2512342372000768E-3</v>
       </c>
     </row>
@@ -4037,17 +4036,17 @@
         <v>515</v>
       </c>
       <c r="B104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30900</v>
       </c>
       <c r="C104">
-        <f t="shared" si="6"/>
+        <f>B104/MAX(B:B)</f>
         <v>0.73049645390070927</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104">
         <v>205.61</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104">
         <v>100</v>
       </c>
       <c r="F104">
@@ -4063,7 +4062,7 @@
         <v>1</v>
       </c>
       <c r="J104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2297143275229869E-3</v>
       </c>
     </row>
@@ -4072,17 +4071,17 @@
         <v>520</v>
       </c>
       <c r="B105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31200</v>
       </c>
       <c r="C105">
-        <f t="shared" si="6"/>
+        <f>B105/MAX(B:B)</f>
         <v>0.73758865248226946</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105">
         <v>204.05</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105">
         <v>100</v>
       </c>
       <c r="F105">
@@ -4098,7 +4097,7 @@
         <v>1</v>
       </c>
       <c r="J105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2052099048249863E-3</v>
       </c>
     </row>
@@ -4107,17 +4106,17 @@
         <v>525</v>
       </c>
       <c r="B106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31500</v>
       </c>
       <c r="C106">
-        <f t="shared" si="6"/>
+        <f>B106/MAX(B:B)</f>
         <v>0.74468085106382975</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106">
         <v>203.51</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106">
         <v>100</v>
       </c>
       <c r="F106">
@@ -4133,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="J106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.196727604660294E-3</v>
       </c>
     </row>
@@ -4142,17 +4141,17 @@
         <v>530</v>
       </c>
       <c r="B107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31800</v>
       </c>
       <c r="C107">
-        <f t="shared" si="6"/>
+        <f>B107/MAX(B:B)</f>
         <v>0.75177304964539005</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107">
         <v>202.04</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107">
         <v>100</v>
       </c>
       <c r="F107">
@@ -4168,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="J107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.1736368986564089E-3</v>
       </c>
     </row>
@@ -4177,17 +4176,17 @@
         <v>535</v>
       </c>
       <c r="B108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32100</v>
       </c>
       <c r="C108">
-        <f t="shared" si="6"/>
+        <f>B108/MAX(B:B)</f>
         <v>0.75886524822695034</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108">
         <v>201.04</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108">
         <v>100</v>
       </c>
       <c r="F108">
@@ -4203,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="J108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.1579289353884598E-3</v>
       </c>
     </row>
@@ -4212,17 +4211,17 @@
         <v>540</v>
       </c>
       <c r="B109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32400</v>
       </c>
       <c r="C109">
-        <f t="shared" si="6"/>
+        <f>B109/MAX(B:B)</f>
         <v>0.76595744680851063</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109">
         <v>199.93</v>
       </c>
-      <c r="E109" s="1">
+      <c r="E109">
         <v>100</v>
       </c>
       <c r="F109">
@@ -4238,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="J109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.1404930961610369E-3</v>
       </c>
     </row>
@@ -4247,17 +4246,17 @@
         <v>545</v>
       </c>
       <c r="B110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32700</v>
       </c>
       <c r="C110">
-        <f t="shared" si="6"/>
+        <f>B110/MAX(B:B)</f>
         <v>0.77304964539007093</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110">
         <v>198.37</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110">
         <v>100</v>
       </c>
       <c r="F110">
@@ -4273,7 +4272,7 @@
         <v>1</v>
       </c>
       <c r="J110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.1159886734630363E-3</v>
       </c>
     </row>
@@ -4282,17 +4281,17 @@
         <v>550</v>
       </c>
       <c r="B111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33000</v>
       </c>
       <c r="C111">
-        <f t="shared" si="6"/>
+        <f>B111/MAX(B:B)</f>
         <v>0.78014184397163122</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111">
         <v>197.53</v>
       </c>
-      <c r="E111" s="1">
+      <c r="E111">
         <v>100</v>
       </c>
       <c r="F111">
@@ -4308,7 +4307,7 @@
         <v>1</v>
       </c>
       <c r="J111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.1027939843179591E-3</v>
       </c>
     </row>
@@ -4317,17 +4316,17 @@
         <v>555</v>
       </c>
       <c r="B112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33300</v>
       </c>
       <c r="C112">
-        <f t="shared" si="6"/>
+        <f>B112/MAX(B:B)</f>
         <v>0.78723404255319152</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112">
         <v>196.37</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E112">
         <v>100</v>
       </c>
       <c r="F112">
@@ -4343,7 +4342,7 @@
         <v>1</v>
       </c>
       <c r="J112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.084572746927138E-3</v>
       </c>
     </row>
@@ -4352,17 +4351,17 @@
         <v>560</v>
       </c>
       <c r="B113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33600</v>
       </c>
       <c r="C113">
-        <f t="shared" si="6"/>
+        <f>B113/MAX(B:B)</f>
         <v>0.79432624113475181</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113">
         <v>195.37</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E113">
         <v>100</v>
       </c>
       <c r="F113">
@@ -4378,7 +4377,7 @@
         <v>1</v>
       </c>
       <c r="J113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.0688647836591898E-3</v>
       </c>
     </row>
@@ -4387,17 +4386,17 @@
         <v>565</v>
       </c>
       <c r="B114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33900</v>
       </c>
       <c r="C114">
-        <f t="shared" si="6"/>
+        <f>B114/MAX(B:B)</f>
         <v>0.8014184397163121</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114">
         <v>194.38</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114">
         <v>100</v>
       </c>
       <c r="F114">
@@ -4413,7 +4412,7 @@
         <v>1</v>
       </c>
       <c r="J114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.0533139000239197E-3</v>
       </c>
     </row>
@@ -4422,17 +4421,17 @@
         <v>570</v>
       </c>
       <c r="B115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34200</v>
       </c>
       <c r="C115">
-        <f t="shared" si="6"/>
+        <f>B115/MAX(B:B)</f>
         <v>0.80851063829787229</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115">
         <v>193.78</v>
       </c>
-      <c r="E115" s="1">
+      <c r="E115">
         <v>100</v>
       </c>
       <c r="F115">
@@ -4448,7 +4447,7 @@
         <v>1</v>
       </c>
       <c r="J115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.0438891220631505E-3</v>
       </c>
     </row>
@@ -4457,17 +4456,17 @@
         <v>575</v>
       </c>
       <c r="B116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34500</v>
       </c>
       <c r="C116">
-        <f t="shared" si="6"/>
+        <f>B116/MAX(B:B)</f>
         <v>0.81560283687943258</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116">
         <v>192.46</v>
       </c>
-      <c r="E116" s="1">
+      <c r="E116">
         <v>100</v>
       </c>
       <c r="F116">
@@ -4483,7 +4482,7 @@
         <v>1</v>
       </c>
       <c r="J116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.0231546105494579E-3</v>
       </c>
     </row>
@@ -4492,17 +4491,17 @@
         <v>580</v>
       </c>
       <c r="B117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34800</v>
       </c>
       <c r="C117">
-        <f t="shared" si="6"/>
+        <f>B117/MAX(B:B)</f>
         <v>0.82269503546099287</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117">
         <v>192.01</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E117">
         <v>100</v>
       </c>
       <c r="F117">
@@ -4518,7 +4517,7 @@
         <v>1</v>
       </c>
       <c r="J117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.0160860270788807E-3</v>
       </c>
     </row>
@@ -4527,17 +4526,17 @@
         <v>585</v>
       </c>
       <c r="B118">
-        <f t="shared" ref="B118:B181" si="7">A118*60</f>
+        <f t="shared" ref="B118:B142" si="5">A118*60</f>
         <v>35100</v>
       </c>
       <c r="C118">
-        <f t="shared" si="6"/>
+        <f>B118/MAX(B:B)</f>
         <v>0.82978723404255317</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118">
         <v>191.56</v>
       </c>
-      <c r="E118" s="1">
+      <c r="E118">
         <v>100</v>
       </c>
       <c r="F118">
@@ -4553,7 +4552,7 @@
         <v>1</v>
       </c>
       <c r="J118">
-        <f t="shared" ref="J118:J181" si="8">1*PI()*H118^4*D118/2/G118</f>
+        <f t="shared" ref="J118:J142" si="6">1*PI()*H118^4*D118/2/G118</f>
         <v>3.0090174436083034E-3</v>
       </c>
     </row>
@@ -4562,33 +4561,33 @@
         <v>590</v>
       </c>
       <c r="B119">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>35400</v>
       </c>
       <c r="C119">
+        <f>B119/MAX(B:B)</f>
+        <v>0.83687943262411346</v>
+      </c>
+      <c r="D119">
+        <v>190.36</v>
+      </c>
+      <c r="E119">
+        <v>100</v>
+      </c>
+      <c r="F119">
+        <v>120</v>
+      </c>
+      <c r="G119">
+        <v>1E-3</v>
+      </c>
+      <c r="H119">
+        <v>0.01</v>
+      </c>
+      <c r="I119">
+        <v>1</v>
+      </c>
+      <c r="J119">
         <f t="shared" si="6"/>
-        <v>0.83687943262411346</v>
-      </c>
-      <c r="D119" s="1">
-        <v>190.36</v>
-      </c>
-      <c r="E119" s="1">
-        <v>100</v>
-      </c>
-      <c r="F119">
-        <v>120</v>
-      </c>
-      <c r="G119">
-        <v>1E-3</v>
-      </c>
-      <c r="H119">
-        <v>0.01</v>
-      </c>
-      <c r="I119">
-        <v>1</v>
-      </c>
-      <c r="J119">
-        <f t="shared" si="8"/>
         <v>2.9901678876867654E-3</v>
       </c>
     </row>
@@ -4597,33 +4596,33 @@
         <v>595</v>
       </c>
       <c r="B120">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>35700</v>
       </c>
       <c r="C120">
+        <f>B120/MAX(B:B)</f>
+        <v>0.84397163120567376</v>
+      </c>
+      <c r="D120">
+        <v>188.98</v>
+      </c>
+      <c r="E120">
+        <v>100</v>
+      </c>
+      <c r="F120">
+        <v>120</v>
+      </c>
+      <c r="G120">
+        <v>1E-3</v>
+      </c>
+      <c r="H120">
+        <v>0.01</v>
+      </c>
+      <c r="I120">
+        <v>1</v>
+      </c>
+      <c r="J120">
         <f t="shared" si="6"/>
-        <v>0.84397163120567376</v>
-      </c>
-      <c r="D120" s="1">
-        <v>188.98</v>
-      </c>
-      <c r="E120" s="1">
-        <v>100</v>
-      </c>
-      <c r="F120">
-        <v>120</v>
-      </c>
-      <c r="G120">
-        <v>1E-3</v>
-      </c>
-      <c r="H120">
-        <v>0.01</v>
-      </c>
-      <c r="I120">
-        <v>1</v>
-      </c>
-      <c r="J120">
-        <f t="shared" si="8"/>
         <v>2.968490898376995E-3</v>
       </c>
     </row>
@@ -4632,33 +4631,33 @@
         <v>600</v>
       </c>
       <c r="B121">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>36000</v>
       </c>
       <c r="C121">
+        <f>B121/MAX(B:B)</f>
+        <v>0.85106382978723405</v>
+      </c>
+      <c r="D121">
+        <v>188.03</v>
+      </c>
+      <c r="E121">
+        <v>100</v>
+      </c>
+      <c r="F121">
+        <v>120</v>
+      </c>
+      <c r="G121">
+        <v>1E-3</v>
+      </c>
+      <c r="H121">
+        <v>0.01</v>
+      </c>
+      <c r="I121">
+        <v>1</v>
+      </c>
+      <c r="J121">
         <f t="shared" si="6"/>
-        <v>0.85106382978723405</v>
-      </c>
-      <c r="D121" s="1">
-        <v>188.03</v>
-      </c>
-      <c r="E121" s="1">
-        <v>100</v>
-      </c>
-      <c r="F121">
-        <v>120</v>
-      </c>
-      <c r="G121">
-        <v>1E-3</v>
-      </c>
-      <c r="H121">
-        <v>0.01</v>
-      </c>
-      <c r="I121">
-        <v>1</v>
-      </c>
-      <c r="J121">
-        <f t="shared" si="8"/>
         <v>2.9535683332724441E-3</v>
       </c>
     </row>
@@ -4667,33 +4666,33 @@
         <v>605</v>
       </c>
       <c r="B122">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>36300</v>
       </c>
       <c r="C122">
+        <f>B122/MAX(B:B)</f>
+        <v>0.85815602836879434</v>
+      </c>
+      <c r="D122">
+        <v>187.27</v>
+      </c>
+      <c r="E122">
+        <v>100</v>
+      </c>
+      <c r="F122">
+        <v>120</v>
+      </c>
+      <c r="G122">
+        <v>1E-3</v>
+      </c>
+      <c r="H122">
+        <v>0.01</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+      <c r="J122">
         <f t="shared" si="6"/>
-        <v>0.85815602836879434</v>
-      </c>
-      <c r="D122" s="1">
-        <v>187.27</v>
-      </c>
-      <c r="E122" s="1">
-        <v>100</v>
-      </c>
-      <c r="F122">
-        <v>120</v>
-      </c>
-      <c r="G122">
-        <v>1E-3</v>
-      </c>
-      <c r="H122">
-        <v>0.01</v>
-      </c>
-      <c r="I122">
-        <v>1</v>
-      </c>
-      <c r="J122">
-        <f t="shared" si="8"/>
         <v>2.9416302811888029E-3</v>
       </c>
     </row>
@@ -4702,33 +4701,33 @@
         <v>610</v>
       </c>
       <c r="B123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>36600</v>
       </c>
       <c r="C123">
+        <f>B123/MAX(B:B)</f>
+        <v>0.86524822695035464</v>
+      </c>
+      <c r="D123">
+        <v>186.48</v>
+      </c>
+      <c r="E123">
+        <v>100</v>
+      </c>
+      <c r="F123">
+        <v>120</v>
+      </c>
+      <c r="G123">
+        <v>1E-3</v>
+      </c>
+      <c r="H123">
+        <v>0.01</v>
+      </c>
+      <c r="I123">
+        <v>1</v>
+      </c>
+      <c r="J123">
         <f t="shared" si="6"/>
-        <v>0.86524822695035464</v>
-      </c>
-      <c r="D123" s="1">
-        <v>186.48</v>
-      </c>
-      <c r="E123" s="1">
-        <v>100</v>
-      </c>
-      <c r="F123">
-        <v>120</v>
-      </c>
-      <c r="G123">
-        <v>1E-3</v>
-      </c>
-      <c r="H123">
-        <v>0.01</v>
-      </c>
-      <c r="I123">
-        <v>1</v>
-      </c>
-      <c r="J123">
-        <f t="shared" si="8"/>
         <v>2.9292209902071226E-3</v>
       </c>
     </row>
@@ -4737,33 +4736,33 @@
         <v>615</v>
       </c>
       <c r="B124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>36900</v>
       </c>
       <c r="C124">
+        <f>B124/MAX(B:B)</f>
+        <v>0.87234042553191493</v>
+      </c>
+      <c r="D124">
+        <v>185.37</v>
+      </c>
+      <c r="E124">
+        <v>100</v>
+      </c>
+      <c r="F124">
+        <v>120</v>
+      </c>
+      <c r="G124">
+        <v>1E-3</v>
+      </c>
+      <c r="H124">
+        <v>0.01</v>
+      </c>
+      <c r="I124">
+        <v>1</v>
+      </c>
+      <c r="J124">
         <f t="shared" si="6"/>
-        <v>0.87234042553191493</v>
-      </c>
-      <c r="D124" s="1">
-        <v>185.37</v>
-      </c>
-      <c r="E124" s="1">
-        <v>100</v>
-      </c>
-      <c r="F124">
-        <v>120</v>
-      </c>
-      <c r="G124">
-        <v>1E-3</v>
-      </c>
-      <c r="H124">
-        <v>0.01</v>
-      </c>
-      <c r="I124">
-        <v>1</v>
-      </c>
-      <c r="J124">
-        <f t="shared" si="8"/>
         <v>2.9117851509796997E-3</v>
       </c>
     </row>
@@ -4772,33 +4771,33 @@
         <v>620</v>
       </c>
       <c r="B125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>37200</v>
       </c>
       <c r="C125">
+        <f>B125/MAX(B:B)</f>
+        <v>0.87943262411347523</v>
+      </c>
+      <c r="D125">
+        <v>184.39</v>
+      </c>
+      <c r="E125">
+        <v>100</v>
+      </c>
+      <c r="F125">
+        <v>120</v>
+      </c>
+      <c r="G125">
+        <v>1E-3</v>
+      </c>
+      <c r="H125">
+        <v>0.01</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="J125">
         <f t="shared" si="6"/>
-        <v>0.87943262411347523</v>
-      </c>
-      <c r="D125" s="1">
-        <v>184.39</v>
-      </c>
-      <c r="E125" s="1">
-        <v>100</v>
-      </c>
-      <c r="F125">
-        <v>120</v>
-      </c>
-      <c r="G125">
-        <v>1E-3</v>
-      </c>
-      <c r="H125">
-        <v>0.01</v>
-      </c>
-      <c r="I125">
-        <v>1</v>
-      </c>
-      <c r="J125">
-        <f t="shared" si="8"/>
         <v>2.8963913469771093E-3</v>
       </c>
     </row>
@@ -4807,33 +4806,33 @@
         <v>625</v>
       </c>
       <c r="B126">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>37500</v>
       </c>
       <c r="C126">
+        <f>B126/MAX(B:B)</f>
+        <v>0.88652482269503541</v>
+      </c>
+      <c r="D126">
+        <v>183.49</v>
+      </c>
+      <c r="E126">
+        <v>100</v>
+      </c>
+      <c r="F126">
+        <v>120</v>
+      </c>
+      <c r="G126">
+        <v>1E-3</v>
+      </c>
+      <c r="H126">
+        <v>0.01</v>
+      </c>
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="J126">
         <f t="shared" si="6"/>
-        <v>0.88652482269503541</v>
-      </c>
-      <c r="D126" s="1">
-        <v>183.49</v>
-      </c>
-      <c r="E126" s="1">
-        <v>100</v>
-      </c>
-      <c r="F126">
-        <v>120</v>
-      </c>
-      <c r="G126">
-        <v>1E-3</v>
-      </c>
-      <c r="H126">
-        <v>0.01</v>
-      </c>
-      <c r="I126">
-        <v>1</v>
-      </c>
-      <c r="J126">
-        <f t="shared" si="8"/>
         <v>2.8822541800359557E-3</v>
       </c>
     </row>
@@ -4842,33 +4841,33 @@
         <v>630</v>
       </c>
       <c r="B127">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>37800</v>
       </c>
       <c r="C127">
+        <f>B127/MAX(B:B)</f>
+        <v>0.8936170212765957</v>
+      </c>
+      <c r="D127">
+        <v>183.1</v>
+      </c>
+      <c r="E127">
+        <v>100</v>
+      </c>
+      <c r="F127">
+        <v>120</v>
+      </c>
+      <c r="G127">
+        <v>1E-3</v>
+      </c>
+      <c r="H127">
+        <v>0.01</v>
+      </c>
+      <c r="I127">
+        <v>1</v>
+      </c>
+      <c r="J127">
         <f t="shared" si="6"/>
-        <v>0.8936170212765957</v>
-      </c>
-      <c r="D127" s="1">
-        <v>183.1</v>
-      </c>
-      <c r="E127" s="1">
-        <v>100</v>
-      </c>
-      <c r="F127">
-        <v>120</v>
-      </c>
-      <c r="G127">
-        <v>1E-3</v>
-      </c>
-      <c r="H127">
-        <v>0.01</v>
-      </c>
-      <c r="I127">
-        <v>1</v>
-      </c>
-      <c r="J127">
-        <f t="shared" si="8"/>
         <v>2.8761280743614553E-3</v>
       </c>
     </row>
@@ -4877,33 +4876,33 @@
         <v>635</v>
       </c>
       <c r="B128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>38100</v>
       </c>
       <c r="C128">
+        <f>B128/MAX(B:B)</f>
+        <v>0.900709219858156</v>
+      </c>
+      <c r="D128">
+        <v>182.76</v>
+      </c>
+      <c r="E128">
+        <v>100</v>
+      </c>
+      <c r="F128">
+        <v>120</v>
+      </c>
+      <c r="G128">
+        <v>1E-3</v>
+      </c>
+      <c r="H128">
+        <v>0.01</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128">
         <f t="shared" si="6"/>
-        <v>0.900709219858156</v>
-      </c>
-      <c r="D128" s="1">
-        <v>182.76</v>
-      </c>
-      <c r="E128" s="1">
-        <v>100</v>
-      </c>
-      <c r="F128">
-        <v>120</v>
-      </c>
-      <c r="G128">
-        <v>1E-3</v>
-      </c>
-      <c r="H128">
-        <v>0.01</v>
-      </c>
-      <c r="I128">
-        <v>1</v>
-      </c>
-      <c r="J128">
-        <f t="shared" si="8"/>
         <v>2.8707873668503527E-3</v>
       </c>
     </row>
@@ -4912,33 +4911,33 @@
         <v>640</v>
       </c>
       <c r="B129">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>38400</v>
       </c>
       <c r="C129">
+        <f>B129/MAX(B:B)</f>
+        <v>0.90780141843971629</v>
+      </c>
+      <c r="D129">
+        <v>181.83</v>
+      </c>
+      <c r="E129">
+        <v>100</v>
+      </c>
+      <c r="F129">
+        <v>120</v>
+      </c>
+      <c r="G129">
+        <v>1E-3</v>
+      </c>
+      <c r="H129">
+        <v>0.01</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="J129">
         <f t="shared" si="6"/>
-        <v>0.90780141843971629</v>
-      </c>
-      <c r="D129" s="1">
-        <v>181.83</v>
-      </c>
-      <c r="E129" s="1">
-        <v>100</v>
-      </c>
-      <c r="F129">
-        <v>120</v>
-      </c>
-      <c r="G129">
-        <v>1E-3</v>
-      </c>
-      <c r="H129">
-        <v>0.01</v>
-      </c>
-      <c r="I129">
-        <v>1</v>
-      </c>
-      <c r="J129">
-        <f t="shared" si="8"/>
         <v>2.8561789610111604E-3</v>
       </c>
     </row>
@@ -4947,33 +4946,33 @@
         <v>645</v>
       </c>
       <c r="B130">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>38700</v>
       </c>
       <c r="C130">
+        <f>B130/MAX(B:B)</f>
+        <v>0.91489361702127658</v>
+      </c>
+      <c r="D130">
+        <v>180.74</v>
+      </c>
+      <c r="E130">
+        <v>100</v>
+      </c>
+      <c r="F130">
+        <v>120</v>
+      </c>
+      <c r="G130">
+        <v>1E-3</v>
+      </c>
+      <c r="H130">
+        <v>0.01</v>
+      </c>
+      <c r="I130">
+        <v>1</v>
+      </c>
+      <c r="J130">
         <f t="shared" si="6"/>
-        <v>0.91489361702127658</v>
-      </c>
-      <c r="D130" s="1">
-        <v>180.74</v>
-      </c>
-      <c r="E130" s="1">
-        <v>100</v>
-      </c>
-      <c r="F130">
-        <v>120</v>
-      </c>
-      <c r="G130">
-        <v>1E-3</v>
-      </c>
-      <c r="H130">
-        <v>0.01</v>
-      </c>
-      <c r="I130">
-        <v>1</v>
-      </c>
-      <c r="J130">
-        <f t="shared" si="8"/>
         <v>2.8390572810490962E-3</v>
       </c>
     </row>
@@ -4982,17 +4981,17 @@
         <v>650</v>
       </c>
       <c r="B131">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39000</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C194" si="9">B131/MAX(B:B)</f>
+        <f>B131/MAX(B:B)</f>
         <v>0.92198581560283688</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D131">
         <v>179.37</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131">
         <v>100</v>
       </c>
       <c r="F131">
@@ -5008,7 +5007,7 @@
         <v>1</v>
       </c>
       <c r="J131">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.8175373713720062E-3</v>
       </c>
     </row>
@@ -5017,17 +5016,17 @@
         <v>655</v>
       </c>
       <c r="B132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39300</v>
       </c>
       <c r="C132">
-        <f t="shared" si="9"/>
+        <f>B132/MAX(B:B)</f>
         <v>0.92907801418439717</v>
       </c>
-      <c r="D132" s="1">
+      <c r="D132">
         <v>179.04</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132">
         <v>100</v>
       </c>
       <c r="F132">
@@ -5043,7 +5042,7 @@
         <v>1</v>
       </c>
       <c r="J132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.8123537434935827E-3</v>
       </c>
     </row>
@@ -5052,17 +5051,17 @@
         <v>660</v>
       </c>
       <c r="B133">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39600</v>
       </c>
       <c r="C133">
-        <f t="shared" si="9"/>
+        <f>B133/MAX(B:B)</f>
         <v>0.93617021276595747</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133">
         <v>178.47</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133">
         <v>100</v>
       </c>
       <c r="F133">
@@ -5078,7 +5077,7 @@
         <v>1</v>
       </c>
       <c r="J133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.8034002044308517E-3</v>
       </c>
     </row>
@@ -5087,17 +5086,17 @@
         <v>665</v>
       </c>
       <c r="B134">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39900</v>
       </c>
       <c r="C134">
-        <f t="shared" si="9"/>
+        <f>B134/MAX(B:B)</f>
         <v>0.94326241134751776</v>
       </c>
-      <c r="D134" s="1">
+      <c r="D134">
         <v>178.05</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134">
         <v>100</v>
       </c>
       <c r="F134">
@@ -5113,7 +5112,7 @@
         <v>1</v>
       </c>
       <c r="J134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.7968028598583136E-3</v>
       </c>
     </row>
@@ -5122,17 +5121,17 @@
         <v>670</v>
       </c>
       <c r="B135">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>40200</v>
       </c>
       <c r="C135">
-        <f t="shared" si="9"/>
+        <f>B135/MAX(B:B)</f>
         <v>0.95035460992907805</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135">
         <v>177.16</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135">
         <v>100</v>
       </c>
       <c r="F135">
@@ -5148,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="J135">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.7828227725498387E-3</v>
       </c>
     </row>
@@ -5157,17 +5156,17 @@
         <v>675</v>
       </c>
       <c r="B136">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>40500</v>
       </c>
       <c r="C136">
-        <f t="shared" si="9"/>
+        <f>B136/MAX(B:B)</f>
         <v>0.95744680851063835</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D136">
         <v>176.26</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136">
         <v>100</v>
       </c>
       <c r="F136">
@@ -5183,7 +5182,7 @@
         <v>1</v>
       </c>
       <c r="J136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.7686856056086846E-3</v>
       </c>
     </row>
@@ -5192,17 +5191,17 @@
         <v>680</v>
       </c>
       <c r="B137">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>40800</v>
       </c>
       <c r="C137">
-        <f t="shared" si="9"/>
+        <f>B137/MAX(B:B)</f>
         <v>0.96453900709219853</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137">
         <v>174.65</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137">
         <v>100</v>
       </c>
       <c r="F137">
@@ -5218,7 +5217,7 @@
         <v>1</v>
       </c>
       <c r="J137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.7433957847472872E-3</v>
       </c>
     </row>
@@ -5227,17 +5226,17 @@
         <v>685</v>
       </c>
       <c r="B138">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>41100</v>
       </c>
       <c r="C138">
-        <f t="shared" si="9"/>
+        <f>B138/MAX(B:B)</f>
         <v>0.97163120567375882</v>
       </c>
-      <c r="D138" s="1">
+      <c r="D138">
         <v>174.38</v>
       </c>
-      <c r="E138" s="1">
+      <c r="E138">
         <v>100</v>
       </c>
       <c r="F138">
@@ -5253,7 +5252,7 @@
         <v>1</v>
       </c>
       <c r="J138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.7391546346649405E-3</v>
       </c>
     </row>
@@ -5262,17 +5261,17 @@
         <v>690</v>
       </c>
       <c r="B139">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>41400</v>
       </c>
       <c r="C139">
-        <f t="shared" si="9"/>
+        <f>B139/MAX(B:B)</f>
         <v>0.97872340425531912</v>
       </c>
-      <c r="D139" s="1">
+      <c r="D139">
         <v>173.78</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139">
         <v>100</v>
       </c>
       <c r="F139">
@@ -5288,7 +5287,7 @@
         <v>1</v>
       </c>
       <c r="J139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.7297298567041713E-3</v>
       </c>
     </row>
@@ -5297,17 +5296,17 @@
         <v>695</v>
       </c>
       <c r="B140">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>41700</v>
       </c>
       <c r="C140">
-        <f t="shared" si="9"/>
+        <f>B140/MAX(B:B)</f>
         <v>0.98581560283687941</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D140">
         <v>171.73</v>
       </c>
-      <c r="E140" s="1">
+      <c r="E140">
         <v>100</v>
       </c>
       <c r="F140">
@@ -5323,7 +5322,7 @@
         <v>1</v>
       </c>
       <c r="J140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.6975285320048757E-3</v>
       </c>
     </row>
@@ -5332,17 +5331,17 @@
         <v>700</v>
       </c>
       <c r="B141">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>42000</v>
       </c>
       <c r="C141">
-        <f t="shared" si="9"/>
+        <f>B141/MAX(B:B)</f>
         <v>0.99290780141843971</v>
       </c>
-      <c r="D141" s="1">
+      <c r="D141">
         <v>170.89</v>
       </c>
-      <c r="E141" s="1">
+      <c r="E141">
         <v>100</v>
       </c>
       <c r="F141">
@@ -5358,7 +5357,7 @@
         <v>1</v>
       </c>
       <c r="J141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.6843338428597986E-3</v>
       </c>
     </row>
@@ -5367,17 +5366,17 @@
         <v>705</v>
       </c>
       <c r="B142">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>42300</v>
       </c>
       <c r="C142">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D142" s="1">
+        <f>B142/MAX(B:B)</f>
+        <v>1</v>
+      </c>
+      <c r="D142">
         <v>170.46</v>
       </c>
-      <c r="E142" s="1">
+      <c r="E142">
         <v>100</v>
       </c>
       <c r="F142">
@@ -5393,7 +5392,7 @@
         <v>1</v>
       </c>
       <c r="J142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.6775794186545809E-3</v>
       </c>
     </row>
@@ -5403,6 +5402,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4BC992AB83A1548A1B8B5F18677A95F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="42d56c5c72d44ab02267f72c956364d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5209e521-73e0-41cd-a274-87675e0c834f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc2d2b1e76373b9f1cfbfa45a89f8b75" ns3:_="">
     <xsd:import namespace="5209e521-73e0-41cd-a274-87675e0c834f"/>
@@ -5554,35 +5568,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0A6231-B768-4D05-9C78-571F4C36A483}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3245B62-6A4A-4085-A048-2914D4991859}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5209e521-73e0-41cd-a274-87675e0c834f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5604,9 +5593,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3245B62-6A4A-4085-A048-2914D4991859}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0A6231-B768-4D05-9C78-571F4C36A483}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5209e521-73e0-41cd-a274-87675e0c834f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>